<commit_message>
Use US EPS values for bldgs/ICpUEfEBE, indst/CoNEPPpCAPS, indst/EoDfIP, indst/ItICM, and trans/RTMF
</commit_message>
<xml_diff>
--- a/InputData/indst/EoDfIP/Elasticities of Demand for Industrial Products.xlsx
+++ b/InputData/indst/EoDfIP/Elasticities of Demand for Industrial Products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\Dropbox (Energy InNovation)\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\indst\EoDfIP (new)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9838DB3E-7439-47D3-9F3C-3145A30A468E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C3777E-C569-4F4C-96CF-4846C77ECCFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="915" windowWidth="24090" windowHeight="16245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="3855" windowWidth="19950" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="87">
   <si>
     <t>Resources for the Future</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>for these particular data.</t>
+  </si>
+  <si>
+    <t>The EU EPS uses values from the US EPS.</t>
   </si>
 </sst>
 </file>
@@ -799,22 +802,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="78.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.59765625" customWidth="1"/>
+    <col min="2" max="2" width="78.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>57</v>
       </c>
@@ -822,64 +827,69 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="3">
         <v>2008</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -897,20 +907,20 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="49.85546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="12" customWidth="1"/>
-    <col min="4" max="16384" width="12.5703125" style="6"/>
+    <col min="1" max="1" width="49.86328125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20.73046875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="35.86328125" style="12" customWidth="1"/>
+    <col min="4" max="16384" width="12.59765625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -921,7 +931,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -932,7 +942,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -943,7 +953,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -954,7 +964,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -965,7 +975,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -976,7 +986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -987,7 +997,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -995,7 +1005,7 @@
         <v>-0.16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
@@ -1006,7 +1016,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
@@ -1017,7 +1027,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
@@ -1028,7 +1038,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
@@ -1039,7 +1049,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
@@ -1050,7 +1060,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
@@ -1061,7 +1071,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
@@ -1072,7 +1082,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
@@ -1083,7 +1093,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
@@ -1094,7 +1104,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
@@ -1105,7 +1115,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
@@ -1116,7 +1126,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
@@ -1127,7 +1137,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -1138,7 +1148,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A23" s="6" t="s">
         <v>23</v>
       </c>
@@ -1149,7 +1159,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -1160,7 +1170,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -1171,7 +1181,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A26" s="6" t="s">
         <v>26</v>
       </c>
@@ -1182,7 +1192,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A27" s="6" t="s">
         <v>27</v>
       </c>
@@ -1193,7 +1203,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A28" s="6" t="s">
         <v>28</v>
       </c>
@@ -1204,7 +1214,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
@@ -1215,7 +1225,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A30" s="6" t="s">
         <v>30</v>
       </c>
@@ -1226,7 +1236,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
@@ -1237,7 +1247,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -1248,7 +1258,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A33" s="6" t="s">
         <v>33</v>
       </c>
@@ -1259,7 +1269,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A34" s="6" t="s">
         <v>34</v>
       </c>
@@ -1270,7 +1280,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A35" s="6" t="s">
         <v>35</v>
       </c>
@@ -1281,7 +1291,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A36" s="6" t="s">
         <v>36</v>
       </c>
@@ -1292,7 +1302,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
@@ -1303,7 +1313,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A38" s="6" t="s">
         <v>38</v>
       </c>
@@ -1314,7 +1324,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A39" s="6" t="s">
         <v>39</v>
       </c>
@@ -1325,7 +1335,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A40" s="6" t="s">
         <v>40</v>
       </c>
@@ -1336,7 +1346,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A41" s="6" t="s">
         <v>41</v>
       </c>
@@ -1347,7 +1357,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A42" s="6" t="s">
         <v>42</v>
       </c>
@@ -1358,7 +1368,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A43" s="6" t="s">
         <v>43</v>
       </c>
@@ -1369,7 +1379,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A44" s="6" t="s">
         <v>44</v>
       </c>
@@ -1380,7 +1390,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A45" s="6" t="s">
         <v>45</v>
       </c>
@@ -1388,7 +1398,7 @@
         <v>-0.745</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
@@ -1396,7 +1406,7 @@
         <v>-0.83299999999999996</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
@@ -1404,7 +1414,7 @@
         <v>-0.83299999999999996</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A48" s="6" t="s">
         <v>48</v>
       </c>
@@ -1412,7 +1422,7 @@
         <v>-0.83299999999999996</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A49" s="6" t="s">
         <v>49</v>
       </c>
@@ -1420,7 +1430,7 @@
         <v>-0.745</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A50" s="6" t="s">
         <v>50</v>
       </c>
@@ -1428,7 +1438,7 @@
         <v>-0.745</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A51" s="6" t="s">
         <v>51</v>
       </c>
@@ -1436,7 +1446,7 @@
         <v>-0.745</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A52" s="6" t="s">
         <v>52</v>
       </c>
@@ -1444,7 +1454,7 @@
         <v>-0.745</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
@@ -1452,7 +1462,7 @@
         <v>-0.745</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
@@ -1472,18 +1482,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="59.42578125" customWidth="1"/>
-    <col min="2" max="4" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="59.3984375" customWidth="1"/>
+    <col min="2" max="4" width="20.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
@@ -1497,7 +1507,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1511,7 +1521,7 @@
         <v>168532</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1525,7 +1535,7 @@
         <v>48460</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1539,7 +1549,7 @@
         <v>126146</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1553,7 +1563,7 @@
         <v>52569</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1567,7 +1577,7 @@
         <v>18881</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1581,7 +1591,7 @@
         <v>56813</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1595,7 +1605,7 @@
         <v>250852</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1609,7 +1619,7 @@
         <v>92926</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1623,7 +1633,7 @@
         <v>1031627</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1637,7 +1647,7 @@
         <v>486680</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1651,7 +1661,7 @@
         <v>62447</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1665,7 +1675,7 @@
         <v>133149</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1679,7 +1689,7 @@
         <v>164005</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1693,7 +1703,7 @@
         <v>5177</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1707,7 +1717,7 @@
         <v>52514</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1721,7 +1731,7 @@
         <v>19882</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1735,7 +1745,7 @@
         <v>145197</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1749,7 +1759,7 @@
         <v>15558</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1763,7 +1773,7 @@
         <v>191641</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -1777,7 +1787,7 @@
         <v>18270</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1791,7 +1801,7 @@
         <v>17745</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1805,7 +1815,7 @@
         <v>47725</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1819,7 +1829,7 @@
         <v>38808</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1833,7 +1843,7 @@
         <v>12508</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1847,7 +1857,7 @@
         <v>9195</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1861,7 +1871,7 @@
         <v>448400</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>73</v>
       </c>
@@ -1875,7 +1885,7 @@
         <v>4861</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1889,7 +1899,7 @@
         <v>8132</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1903,7 +1913,7 @@
         <v>4837</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1917,7 +1927,7 @@
         <v>4787</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1931,7 +1941,7 @@
         <v>74686</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -1945,7 +1955,7 @@
         <v>62903</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -1959,7 +1969,7 @@
         <v>22262</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1973,7 +1983,7 @@
         <v>14545</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1987,7 +1997,7 @@
         <v>11142</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -2001,7 +2011,7 @@
         <v>29823</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -2015,7 +2025,7 @@
         <v>225327</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2029,7 +2039,7 @@
         <v>228125</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2043,7 +2053,7 @@
         <v>466241</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2057,7 +2067,7 @@
         <v>450146</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -2071,7 +2081,7 @@
         <v>105557</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2085,7 +2095,7 @@
         <v>158471</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2099,7 +2109,7 @@
         <v>1645222</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2113,7 +2123,7 @@
         <v>102147</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -2127,7 +2137,7 @@
         <v>187881</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -2141,7 +2151,7 @@
         <v>297242</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -2155,7 +2165,7 @@
         <v>625365</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -2169,7 +2179,7 @@
         <v>1074983</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -2183,7 +2193,7 @@
         <v>1953017</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -2197,7 +2207,7 @@
         <v>1927957</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2211,7 +2221,7 @@
         <v>2729030</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2240,13 +2250,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.86328125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
         <v>69</v>
       </c>
@@ -2254,7 +2264,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -2263,7 +2273,7 @@
         <v>-0.82699999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -2272,7 +2282,7 @@
         <v>-0.26923600535787917</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -2281,7 +2291,7 @@
         <v>-0.95299999999999985</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -2290,7 +2300,7 @@
         <v>-0.98568388783511685</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2299,7 +2309,7 @@
         <v>-0.106</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -2308,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -2317,7 +2327,7 @@
         <v>-0.81200000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
use US data for indst/EoDfIP
</commit_message>
<xml_diff>
--- a/InputData/indst/EoDfIP/Elasticities of Demand for Industrial Products.xlsx
+++ b/InputData/indst/EoDfIP/Elasticities of Demand for Industrial Products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\indst\EoDfIP (new)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\Documents\Energy Policy Simulator\Models\eps-eu\InputData\indst\EoDfIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C3777E-C569-4F4C-96CF-4846C77ECCFD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AF6ADE-F9AB-4F0B-97DE-FCD0244F8413}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="3855" windowWidth="19950" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14130" yWindow="-17025" windowWidth="18390" windowHeight="16365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="105">
   <si>
     <t>Resources for the Future</t>
   </si>
@@ -222,9 +222,6 @@
     <t>Government excluding electricity</t>
   </si>
   <si>
-    <t>Agriculture</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -246,24 +243,6 @@
     <t>https://media.rff.org/documents/RFF-DP-08-37.pdf</t>
   </si>
   <si>
-    <t>Natural gas and petroleum systems</t>
-  </si>
-  <si>
-    <t>Iron and steel</t>
-  </si>
-  <si>
-    <t>Chemicals</t>
-  </si>
-  <si>
-    <t>Other industries</t>
-  </si>
-  <si>
-    <t>Cement and other carbonates</t>
-  </si>
-  <si>
-    <t>Water + waste</t>
-  </si>
-  <si>
     <t>Unit: dimensionless (elasticity)</t>
   </si>
   <si>
@@ -313,6 +292,81 @@
   </si>
   <si>
     <t>for these particular data.</t>
+  </si>
+  <si>
+    <t>agriculture and forestry 01T03</t>
+  </si>
+  <si>
+    <t>coal mining 05</t>
+  </si>
+  <si>
+    <t>oil and gas extraction 06</t>
+  </si>
+  <si>
+    <t>other mining and quarrying 07T08</t>
+  </si>
+  <si>
+    <t>food beverage and tobacco 10T12</t>
+  </si>
+  <si>
+    <t>textiles apparel and leather 13T15</t>
+  </si>
+  <si>
+    <t>wood products 16</t>
+  </si>
+  <si>
+    <t>pulp paper and printing 17T18</t>
+  </si>
+  <si>
+    <t>refined petroleum and coke 19</t>
+  </si>
+  <si>
+    <t>chemicals 20</t>
+  </si>
+  <si>
+    <t>rubber and plastic products 22</t>
+  </si>
+  <si>
+    <t>glass and glass products 231</t>
+  </si>
+  <si>
+    <t>cement and other nonmetallic minerals 239</t>
+  </si>
+  <si>
+    <t>iron and steel 241</t>
+  </si>
+  <si>
+    <t>other metals 242</t>
+  </si>
+  <si>
+    <t>metal products except machinery and vehicles 25</t>
+  </si>
+  <si>
+    <t>computers and electronics 26</t>
+  </si>
+  <si>
+    <t>appliances and electrical equipment 27</t>
+  </si>
+  <si>
+    <t>other machinery 28</t>
+  </si>
+  <si>
+    <t>road vehicles 29</t>
+  </si>
+  <si>
+    <t>nonroad vehicles 30</t>
+  </si>
+  <si>
+    <t>other manufacturing 31T33</t>
+  </si>
+  <si>
+    <t>energy pipelines and gas processing 352T353</t>
+  </si>
+  <si>
+    <t>water and waste 36T39</t>
+  </si>
+  <si>
+    <t>construction 41T43</t>
   </si>
   <si>
     <t>The EU EPS uses values from the US EPS.</t>
@@ -429,7 +483,7 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -460,6 +514,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -805,7 +860,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -816,15 +871,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -844,52 +899,52 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -917,7 +972,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.5">
@@ -925,10 +980,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.5">
@@ -939,7 +994,7 @@
         <v>-0.81200000000000006</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
@@ -950,7 +1005,7 @@
         <v>-0.81200000000000006</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
@@ -961,7 +1016,7 @@
         <v>-0.29599999999999999</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
@@ -972,7 +1027,7 @@
         <v>-0.29599999999999999</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.5">
@@ -983,7 +1038,7 @@
         <v>-0.106</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.5">
@@ -994,7 +1049,7 @@
         <v>-0.63300000000000001</v>
       </c>
       <c r="C8" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.5">
@@ -1013,7 +1068,7 @@
         <v>-0.56599999999999995</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.5">
@@ -1024,7 +1079,7 @@
         <v>-0.77400000000000002</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.5">
@@ -1035,7 +1090,7 @@
         <v>-0.63800000000000001</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.5">
@@ -1046,7 +1101,7 @@
         <v>-1.139</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.5">
@@ -1057,7 +1112,7 @@
         <v>-2.4180000000000001</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.5">
@@ -1068,7 +1123,7 @@
         <v>-0.69799999999999995</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.5">
@@ -1079,7 +1134,7 @@
         <v>-0.69799999999999995</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.5">
@@ -1090,7 +1145,7 @@
         <v>-0.69799999999999995</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.5">
@@ -1101,7 +1156,7 @@
         <v>-0.69799999999999995</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.5">
@@ -1112,7 +1167,7 @@
         <v>-0.69799999999999995</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.5">
@@ -1123,7 +1178,7 @@
         <v>-7.0999999999999994E-2</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.5">
@@ -1134,7 +1189,7 @@
         <v>-7.0999999999999994E-2</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.5">
@@ -1145,7 +1200,7 @@
         <v>-0.98699999999999999</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.5">
@@ -1156,7 +1211,7 @@
         <v>-0.98699999999999999</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.5">
@@ -1167,7 +1222,7 @@
         <v>-0.98699999999999999</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.5">
@@ -1178,7 +1233,7 @@
         <v>-0.98699999999999999</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.5">
@@ -1189,7 +1244,7 @@
         <v>-0.98699999999999999</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.5">
@@ -1200,7 +1255,7 @@
         <v>-0.98699999999999999</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.5">
@@ -1211,7 +1266,7 @@
         <v>-0.98699999999999999</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.5">
@@ -1222,7 +1277,7 @@
         <v>-0.82699999999999996</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.5">
@@ -1233,7 +1288,7 @@
         <v>-0.82699999999999996</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.5">
@@ -1244,7 +1299,7 @@
         <v>-0.82699999999999996</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.5">
@@ -1255,7 +1310,7 @@
         <v>-0.82699999999999996</v>
       </c>
       <c r="C32" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.5">
@@ -1266,7 +1321,7 @@
         <v>-0.82699999999999996</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.5">
@@ -1277,7 +1332,7 @@
         <v>-0.95299999999999996</v>
       </c>
       <c r="C34" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.5">
@@ -1288,7 +1343,7 @@
         <v>-0.95299999999999996</v>
       </c>
       <c r="C35" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.5">
@@ -1299,7 +1354,7 @@
         <v>-0.95299999999999996</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.5">
@@ -1310,7 +1365,7 @@
         <v>-0.95299999999999996</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.5">
@@ -1321,7 +1376,7 @@
         <v>-0.95299999999999996</v>
       </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.5">
@@ -1332,7 +1387,7 @@
         <v>-0.505</v>
       </c>
       <c r="C39" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.5">
@@ -1343,7 +1398,7 @@
         <v>-1.6619999999999999</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.5">
@@ -1354,7 +1409,7 @@
         <v>-2.5960000000000001</v>
       </c>
       <c r="C41" t="s">
-        <v>66</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.5">
@@ -1365,7 +1420,7 @@
         <v>-2.4849999999999999</v>
       </c>
       <c r="C42" t="s">
-        <v>66</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.5">
@@ -1376,7 +1431,7 @@
         <v>-2.4849999999999999</v>
       </c>
       <c r="C43" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.5">
@@ -1387,7 +1442,7 @@
         <v>-1.6619999999999999</v>
       </c>
       <c r="C44" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.5">
@@ -1490,7 +1545,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
@@ -1498,13 +1553,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
@@ -1775,7 +1830,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B22" s="15">
         <v>14743</v>
@@ -1873,7 +1928,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B29" s="15">
         <v>4367</v>
@@ -2125,7 +2180,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B47" s="15">
         <v>194732</v>
@@ -2246,94 +2301,247 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="35.86328125" customWidth="1"/>
+    <col min="1" max="1" width="47.3984375" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="10" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B2" s="11" cm="1">
         <f t="array" ref="B2">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A2),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A2),0)</f>
-        <v>-0.82699999999999996</v>
+        <v>-0.81200000000000006</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B3" s="11" cm="1">
         <f t="array" ref="B3">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A3),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A3),0)</f>
-        <v>-0.26923600535787917</v>
+        <v>-0.106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="B4" s="11" cm="1">
         <f t="array" ref="B4">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A4),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A4),0)</f>
-        <v>-0.95299999999999985</v>
+        <v>-0.29599999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B5" s="11" cm="1">
         <f t="array" ref="B5">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A5),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A5),0)</f>
-        <v>-0.98568388783511685</v>
+        <v>-0.63300000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="B6" s="11" cm="1">
         <f t="array" ref="B6">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A6),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A6),0)</f>
-        <v>-0.106</v>
+        <v>-0.63800000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="B7" s="11" cm="1">
         <f t="array" ref="B7">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A7),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A7),0)</f>
-        <v>0</v>
+        <v>-1.6823913135674904</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="B8" s="11" cm="1">
         <f t="array" ref="B8">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A8),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A8),0)</f>
-        <v>-0.81200000000000006</v>
+        <v>-0.69799999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="B9" s="11" cm="1">
         <f t="array" ref="B9">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A9),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A9),0)</f>
-        <v>-1.2596118059082353</v>
+        <v>-0.69799999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="11" cm="1">
+        <f t="array" ref="B10">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A10),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A10),0)</f>
+        <v>-7.0999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="11" cm="1">
+        <f t="array" ref="B11">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A11),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A11),0)</f>
+        <v>-0.98699999999999988</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="11" cm="1">
+        <f t="array" ref="B12">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A12),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A12),0)</f>
+        <v>-0.98528503405534762</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="18">
+        <f>B14</f>
+        <v>-0.82699999999999985</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="11" cm="1">
+        <f t="array" ref="B14">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A14),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A14),0)</f>
+        <v>-0.82699999999999985</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="11" cm="1">
+        <f t="array" ref="B15">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A15),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A15),0)</f>
+        <v>-0.95299999999999985</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="11" cm="1">
+        <f t="array" ref="B16">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A16),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A16),0)</f>
+        <v>-0.95300000000000007</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="11" cm="1">
+        <f t="array" ref="B17">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A17),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A17),0)</f>
+        <v>-0.505</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="11" cm="1">
+        <f t="array" ref="B18">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A18),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A18),0)</f>
+        <v>-2.5960000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="18">
+        <f>B18</f>
+        <v>-2.5960000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="11" cm="1">
+        <f t="array" ref="B20">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A20),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A20),0)</f>
+        <v>-1.6619999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="11" cm="1">
+        <f t="array" ref="B21">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A21),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A21),0)</f>
+        <v>-2.4849999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" s="11" cm="1">
+        <f t="array" ref="B22">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A22),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A22),0)</f>
+        <v>-2.4849999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="11" cm="1">
+        <f t="array" ref="B23">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A23),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A23),0)</f>
+        <v>-1.6619999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B24" s="11" cm="1">
+        <f t="array" ref="B24">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A24),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A24),0)</f>
+        <v>-0.56599999999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="11" cm="1">
+        <f t="array" ref="B25">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A25),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A25),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="11" cm="1">
+        <f t="array" ref="B26">IFERROR(SUMPRODUCT(--('Table B6'!$C$3:$C$54=$A26),'Table B6'!$B$3:$B$54,'Table A1'!$B$3:$B$54)/SUMIFS('Table A1'!$B$3:$B$54,'Table B6'!$C$3:$C$54,$A26),0)</f>
+        <v>-0.77400000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploading Agora/EI indst and io-model data files
</commit_message>
<xml_diff>
--- a/InputData/indst/EoDfIP/Elasticities of Demand for Industrial Products.xlsx
+++ b/InputData/indst/EoDfIP/Elasticities of Demand for Industrial Products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeRepositories\eps-us\InputData\indst\EoDfIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energyinnovation.sharepoint.com/sites/EUEPSModeling/Shared Documents/InputData_EI+Agora/indst/EoDfIP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22524823-0D3A-4448-8DBE-2DA7964E966A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22524823-0D3A-4448-8DBE-2DA7964E966A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="135" windowWidth="23805" windowHeight="15630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1480" yWindow="1480" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -534,9 +534,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -574,9 +574,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -609,26 +609,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -661,26 +644,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -858,18 +824,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="78.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="2" max="2" width="78.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>56</v>
       </c>
@@ -877,62 +843,62 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>2008</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -952,20 +918,20 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="49.85546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="12" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" style="12" customWidth="1"/>
-    <col min="4" max="16384" width="12.5703125" style="6"/>
+    <col min="1" max="1" width="49.81640625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="35.81640625" style="12" customWidth="1"/>
+    <col min="4" max="16384" width="12.54296875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -976,7 +942,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
@@ -987,7 +953,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
@@ -998,7 +964,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1009,7 +975,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -1020,7 +986,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -1031,7 +997,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -1042,7 +1008,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -1050,7 +1016,7 @@
         <v>-0.16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>6</v>
       </c>
@@ -1061,7 +1027,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
@@ -1072,7 +1038,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
@@ -1083,7 +1049,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
@@ -1094,7 +1060,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
@@ -1105,7 +1071,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
@@ -1116,7 +1082,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
@@ -1127,7 +1093,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
@@ -1138,7 +1104,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
@@ -1149,7 +1115,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
@@ -1160,7 +1126,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
@@ -1171,7 +1137,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
@@ -1182,7 +1148,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
@@ -1193,7 +1159,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>23</v>
       </c>
@@ -1204,7 +1170,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
@@ -1215,7 +1181,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>25</v>
       </c>
@@ -1226,7 +1192,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
         <v>26</v>
       </c>
@@ -1237,7 +1203,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="6" t="s">
         <v>27</v>
       </c>
@@ -1248,7 +1214,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="6" t="s">
         <v>28</v>
       </c>
@@ -1259,7 +1225,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>29</v>
       </c>
@@ -1270,7 +1236,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="6" t="s">
         <v>30</v>
       </c>
@@ -1281,7 +1247,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>31</v>
       </c>
@@ -1292,7 +1258,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -1303,7 +1269,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="6" t="s">
         <v>33</v>
       </c>
@@ -1314,7 +1280,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="6" t="s">
         <v>34</v>
       </c>
@@ -1325,7 +1291,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="6" t="s">
         <v>35</v>
       </c>
@@ -1336,7 +1302,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="6" t="s">
         <v>36</v>
       </c>
@@ -1347,7 +1313,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
@@ -1358,7 +1324,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>38</v>
       </c>
@@ -1369,7 +1335,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="6" t="s">
         <v>39</v>
       </c>
@@ -1380,7 +1346,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="6" t="s">
         <v>40</v>
       </c>
@@ -1391,7 +1357,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="6" t="s">
         <v>41</v>
       </c>
@@ -1402,7 +1368,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="6" t="s">
         <v>42</v>
       </c>
@@ -1413,7 +1379,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="6" t="s">
         <v>43</v>
       </c>
@@ -1424,7 +1390,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="6" t="s">
         <v>44</v>
       </c>
@@ -1435,7 +1401,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="6" t="s">
         <v>45</v>
       </c>
@@ -1443,7 +1409,7 @@
         <v>-0.745</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
         <v>46</v>
       </c>
@@ -1451,7 +1417,7 @@
         <v>-0.83299999999999996</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="6" t="s">
         <v>47</v>
       </c>
@@ -1459,7 +1425,7 @@
         <v>-0.83299999999999996</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="6" t="s">
         <v>48</v>
       </c>
@@ -1467,7 +1433,7 @@
         <v>-0.83299999999999996</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="6" t="s">
         <v>49</v>
       </c>
@@ -1475,7 +1441,7 @@
         <v>-0.745</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>50</v>
       </c>
@@ -1483,7 +1449,7 @@
         <v>-0.745</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>51</v>
       </c>
@@ -1491,7 +1457,7 @@
         <v>-0.745</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="6" t="s">
         <v>52</v>
       </c>
@@ -1499,7 +1465,7 @@
         <v>-0.745</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
@@ -1507,7 +1473,7 @@
         <v>-0.745</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="6" t="s">
         <v>54</v>
       </c>
@@ -1527,18 +1493,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="59.42578125" customWidth="1"/>
-    <col min="2" max="4" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="59.453125" customWidth="1"/>
+    <col min="2" max="4" width="20.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
@@ -1552,7 +1518,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1566,7 +1532,7 @@
         <v>168532</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1580,7 +1546,7 @@
         <v>48460</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1594,7 +1560,7 @@
         <v>126146</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1608,7 +1574,7 @@
         <v>52569</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1622,7 +1588,7 @@
         <v>18881</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1636,7 +1602,7 @@
         <v>56813</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1650,7 +1616,7 @@
         <v>250852</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1664,7 +1630,7 @@
         <v>92926</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1678,7 +1644,7 @@
         <v>1031627</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1692,7 +1658,7 @@
         <v>486680</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1706,7 +1672,7 @@
         <v>62447</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1720,7 +1686,7 @@
         <v>133149</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1734,7 +1700,7 @@
         <v>164005</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1748,7 +1714,7 @@
         <v>5177</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1762,7 +1728,7 @@
         <v>52514</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1776,7 +1742,7 @@
         <v>19882</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1790,7 +1756,7 @@
         <v>145197</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1804,7 +1770,7 @@
         <v>15558</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1818,7 +1784,7 @@
         <v>191641</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -1832,7 +1798,7 @@
         <v>18270</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1846,7 +1812,7 @@
         <v>17745</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1860,7 +1826,7 @@
         <v>47725</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1874,7 +1840,7 @@
         <v>38808</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1888,7 +1854,7 @@
         <v>12508</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1902,7 +1868,7 @@
         <v>9195</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1916,7 +1882,7 @@
         <v>448400</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -1930,7 +1896,7 @@
         <v>4861</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1944,7 +1910,7 @@
         <v>8132</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1958,7 +1924,7 @@
         <v>4837</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -1972,7 +1938,7 @@
         <v>4787</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1986,7 +1952,7 @@
         <v>74686</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -2000,7 +1966,7 @@
         <v>62903</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -2014,7 +1980,7 @@
         <v>22262</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2028,7 +1994,7 @@
         <v>14545</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2042,7 +2008,7 @@
         <v>11142</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -2056,7 +2022,7 @@
         <v>29823</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -2070,7 +2036,7 @@
         <v>225327</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -2084,7 +2050,7 @@
         <v>228125</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -2098,7 +2064,7 @@
         <v>466241</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -2112,7 +2078,7 @@
         <v>450146</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -2126,7 +2092,7 @@
         <v>105557</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -2140,7 +2106,7 @@
         <v>158471</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -2154,7 +2120,7 @@
         <v>1645222</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -2168,7 +2134,7 @@
         <v>102147</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>67</v>
       </c>
@@ -2182,7 +2148,7 @@
         <v>187881</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -2196,7 +2162,7 @@
         <v>297242</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -2210,7 +2176,7 @@
         <v>625365</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -2224,7 +2190,7 @@
         <v>1074983</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -2238,7 +2204,7 @@
         <v>1953017</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -2252,7 +2218,7 @@
         <v>1927957</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -2266,7 +2232,7 @@
         <v>2729030</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -2295,13 +2261,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" customWidth="1"/>
+    <col min="1" max="1" width="47.453125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>62</v>
       </c>
@@ -2309,7 +2275,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -2318,7 +2284,7 @@
         <v>-0.81200000000000006</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -2327,7 +2293,7 @@
         <v>-0.106</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -2336,7 +2302,7 @@
         <v>-0.29599999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -2345,7 +2311,7 @@
         <v>-0.63300000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -2354,7 +2320,7 @@
         <v>-0.63800000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -2363,7 +2329,7 @@
         <v>-1.6823913135674904</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -2372,7 +2338,7 @@
         <v>-0.69799999999999995</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -2381,7 +2347,7 @@
         <v>-0.69799999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -2390,7 +2356,7 @@
         <v>-7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -2399,7 +2365,7 @@
         <v>-0.98699999999999988</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -2408,7 +2374,7 @@
         <v>-0.98528503405534762</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>90</v>
       </c>
@@ -2417,7 +2383,7 @@
         <v>-0.82699999999999985</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -2426,7 +2392,7 @@
         <v>-0.82699999999999985</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>92</v>
       </c>
@@ -2435,7 +2401,7 @@
         <v>-0.95299999999999985</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -2444,7 +2410,7 @@
         <v>-0.95300000000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>94</v>
       </c>
@@ -2453,7 +2419,7 @@
         <v>-0.505</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>95</v>
       </c>
@@ -2462,7 +2428,7 @@
         <v>-2.5960000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>96</v>
       </c>
@@ -2471,7 +2437,7 @@
         <v>-2.5960000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>97</v>
       </c>
@@ -2480,7 +2446,7 @@
         <v>-1.6619999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>98</v>
       </c>
@@ -2489,7 +2455,7 @@
         <v>-2.4849999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>99</v>
       </c>
@@ -2498,7 +2464,7 @@
         <v>-2.4849999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>100</v>
       </c>
@@ -2507,7 +2473,7 @@
         <v>-1.6619999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>101</v>
       </c>
@@ -2516,7 +2482,7 @@
         <v>-0.56599999999999995</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>102</v>
       </c>
@@ -2525,7 +2491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>103</v>
       </c>
@@ -2538,4 +2504,285 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A08BDF573E2FFD46A5F05DED9AF68025" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f85c0eb68479ad8b8987805fd5b8836b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00484652-42e1-479e-92f4-fb0efddcdf60" xmlns:ns3="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7dbc72841229da9eaa30ebb1456cd70" ns2:_="" ns3:_="">
+    <xsd:import namespace="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <xsd:import namespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="00484652-42e1-479e-92f4-fb0efddcdf60" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="12" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="eca5b831-c3dc-41cf-bd85-218b82cecb21" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="16" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="13" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{c5b79d03-3bfd-4c46-9947-056a2403f6c9}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="19" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="20" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{796A7F67-B1F1-4569-A7F0-7BB5082B3550}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0F187C4-83F1-42D9-9DB4-F24DAF094D9B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{100C5935-0C1B-4C3F-B3BD-724D368C8C53}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>